<commit_message>
Korrekturen Natasa und Roger eingetragen
</commit_message>
<xml_diff>
--- a/DataDictionary/Crosswalk.xlsx
+++ b/DataDictionary/Crosswalk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarjan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\xIsadg\01_workbench\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$I$71</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -1784,7 +1787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1828,15 +1831,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1875,9 +1872,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2148,21 +2142,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.625" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.25" style="10" customWidth="1"/>
-    <col min="3" max="3" width="4.75" style="19" customWidth="1"/>
+    <col min="3" max="3" width="4.75" style="17" customWidth="1"/>
     <col min="4" max="4" width="26.375" style="10" customWidth="1"/>
     <col min="5" max="5" width="24.25" style="10" customWidth="1"/>
     <col min="6" max="6" width="56.375" style="1" customWidth="1"/>
@@ -2193,7 +2184,7 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="2"/>
@@ -2204,7 +2195,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="20">
+      <c r="C3" s="18">
         <v>1.1000000000000001</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -2227,7 +2218,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="20">
+      <c r="C4" s="18">
         <v>1.2</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -2250,7 +2241,7 @@
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="20">
+      <c r="C5" s="18">
         <v>1.3</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -2265,7 +2256,7 @@
     <row r="6" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="23"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="9"/>
       <c r="E6" s="13" t="s">
         <v>64</v>
@@ -2284,9 +2275,9 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="23"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="22" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="2"/>
@@ -2297,9 +2288,9 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="23"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="2"/>
@@ -2310,9 +2301,9 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="23"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="24" t="s">
         <v>66</v>
       </c>
       <c r="F9" s="2"/>
@@ -2323,9 +2314,9 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="23"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="24" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="2"/>
@@ -2336,10 +2327,10 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="27">
+      <c r="C11" s="25">
         <v>1.4</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="6"/>
@@ -2359,7 +2350,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="27">
+      <c r="C12" s="25">
         <v>1.5</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -2374,7 +2365,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="22"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="9"/>
       <c r="E13" s="14" t="s">
         <v>41</v>
@@ -2389,9 +2380,9 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="22"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="26" t="s">
         <v>42</v>
       </c>
       <c r="F14" s="2"/>
@@ -2419,7 +2410,7 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C17" s="20">
+      <c r="C17" s="18">
         <v>2.1</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2436,7 +2427,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C18" s="20">
+      <c r="C18" s="18">
         <v>2.2000000000000002</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -2451,8 +2442,8 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="C19" s="20">
+      <c r="A19" s="17"/>
+      <c r="C19" s="18">
         <v>2.2999999999999998</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2465,7 +2456,7 @@
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C20" s="20">
+      <c r="C20" s="18">
         <v>2.4</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -2498,7 +2489,7 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C23" s="27">
+      <c r="C23" s="25">
         <v>3.1</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2510,7 +2501,7 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C24" s="29"/>
+      <c r="C24" s="27"/>
       <c r="E24" s="15" t="s">
         <v>43</v>
       </c>
@@ -2524,8 +2515,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C25" s="30"/>
-      <c r="E25" s="17" t="s">
+      <c r="C25" s="28"/>
+      <c r="E25" s="14" t="s">
         <v>44</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -2538,7 +2529,7 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C26" s="27">
+      <c r="C26" s="25">
         <v>3.2</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -2553,7 +2544,7 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C27" s="27">
+      <c r="C27" s="25">
         <v>3.3</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2566,7 +2557,7 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C28" s="27">
+      <c r="C28" s="25">
         <v>3.4</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -2600,7 +2591,7 @@
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C31" s="20">
+      <c r="C31" s="18">
         <v>4.0999999999999996</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2613,9 +2604,9 @@
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C32" s="29"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="9"/>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F32" s="2"/>
@@ -2630,7 +2621,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C33" s="23"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="9"/>
       <c r="E33" s="15" t="s">
         <v>46</v>
@@ -2647,7 +2638,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="23"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="9"/>
       <c r="E34" s="15" t="s">
         <v>47</v>
@@ -2664,9 +2655,9 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="23"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F35" s="2"/>
@@ -2681,9 +2672,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="23"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="9"/>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F36" s="2"/>
@@ -2698,7 +2689,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="23"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="2"/>
@@ -2707,7 +2698,7 @@
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C38" s="20">
+      <c r="C38" s="18">
         <v>4.2</v>
       </c>
       <c r="D38" s="6" t="s">
@@ -2720,7 +2711,7 @@
       <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C39" s="20">
+      <c r="C39" s="18">
         <v>4.3</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -2733,10 +2724,10 @@
       <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C40" s="20">
+      <c r="C40" s="18">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E40" s="9"/>
@@ -2750,7 +2741,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C41" s="20">
+      <c r="C41" s="18">
         <v>4.5</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -2783,7 +2774,7 @@
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C44" s="27">
+      <c r="C44" s="25">
         <v>5.0999999999999996</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -2795,7 +2786,7 @@
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C45" s="27">
+      <c r="C45" s="25">
         <v>5.2</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2807,7 +2798,7 @@
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C46" s="27">
+      <c r="C46" s="25">
         <v>5.3</v>
       </c>
       <c r="D46" s="6" t="s">
@@ -2819,7 +2810,7 @@
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C47" s="27">
+      <c r="C47" s="25">
         <v>5.4</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -2853,7 +2844,7 @@
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="20">
+      <c r="C50" s="18">
         <v>6.1</v>
       </c>
       <c r="D50" s="6" t="s">
@@ -2894,7 +2885,7 @@
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C53" s="20">
+      <c r="C53" s="18">
         <v>7.1</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2907,7 +2898,7 @@
       <c r="I53" s="2"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C54" s="20">
+      <c r="C54" s="18">
         <v>7.2</v>
       </c>
       <c r="D54" s="6" t="s">
@@ -2920,7 +2911,7 @@
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C55" s="20">
+      <c r="C55" s="18">
         <v>7.3</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -2945,7 +2936,7 @@
       <c r="B57" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="27"/>
+      <c r="C57" s="25"/>
       <c r="D57" s="6"/>
       <c r="E57" s="9"/>
       <c r="F57" s="2"/>
@@ -2954,7 +2945,7 @@
       <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="C58" s="27"/>
+      <c r="C58" s="25"/>
       <c r="D58" s="6" t="s">
         <v>35</v>
       </c>
@@ -2967,7 +2958,7 @@
       <c r="I58" s="2"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C59" s="27"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="14" t="s">
         <v>36</v>
       </c>
@@ -2987,7 +2978,7 @@
       <c r="B61" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="22"/>
+      <c r="C61" s="20"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="11"/>
@@ -2996,7 +2987,7 @@
       <c r="I61" s="11"/>
     </row>
     <row r="62" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C62" s="27"/>
+      <c r="C62" s="25"/>
       <c r="D62" s="6" t="s">
         <v>37</v>
       </c>
@@ -3007,7 +2998,7 @@
       <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" ht="286.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C63" s="22"/>
+      <c r="C63" s="20"/>
       <c r="E63" s="6" t="s">
         <v>50</v>
       </c>
@@ -3017,28 +3008,28 @@
       <c r="G63" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="H63" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="I63" s="21" t="s">
+      <c r="I63" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C64" s="22"/>
+      <c r="C64" s="20"/>
       <c r="E64" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C65" s="27"/>
+      <c r="C65" s="25"/>
       <c r="D65" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E65" s="6"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D68" s="32" t="s">
+      <c r="D68" s="29" t="s">
         <v>61</v>
       </c>
       <c r="E68" s="10" t="s">
@@ -3046,8 +3037,8 @@
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B69" s="33"/>
-      <c r="D69" s="33" t="s">
+      <c r="B69" s="30"/>
+      <c r="D69" s="30" t="s">
         <v>56</v>
       </c>
       <c r="E69" s="10" t="s">
@@ -3055,7 +3046,7 @@
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D70" s="18" t="s">
+      <c r="D70" s="16" t="s">
         <v>57</v>
       </c>
       <c r="E70" s="10" t="s">
@@ -3063,10 +3054,10 @@
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D71" s="34" t="s">
+      <c r="D71" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E71" s="35" t="s">
+      <c r="E71" s="32" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3076,8 +3067,8 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="56" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>